<commit_message>
QA Regression Fixes for duplicate records story change
</commit_message>
<xml_diff>
--- a/data/BuildingPermit/SanMateoBuildingPermits/NonNumericValueSanMateo.xlsx
+++ b/data/BuildingPermit/SanMateoBuildingPermits/NonNumericValueSanMateo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikjain2\Documents\SanMateo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikjain2\SanMateo\Project\pre-release\qa_automation\data\BuildingPermit\SanMateoBuildingPermits\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
   <si>
     <t>CITYCODE</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>NonNumeric</t>
+  </si>
+  <si>
+    <t>BD-2018-888894</t>
   </si>
 </sst>
 </file>
@@ -621,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1203,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C8" s="9">
         <v>43133</v>

</xml_diff>

<commit_message>
Changes for SMAB-3385 and smoke fix for one Building Permit Test case
</commit_message>
<xml_diff>
--- a/data/BuildingPermit/SanMateoBuildingPermits/NonNumericValueSanMateo.xlsx
+++ b/data/BuildingPermit/SanMateoBuildingPermits/NonNumericValueSanMateo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikjain2\SanMateo\Project\pre-release\qa_automation\data\BuildingPermit\SanMateoBuildingPermits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikjain2\SanMateo\Project\APAS_Automation_NJ\qa_automation\data\BuildingPermit\SanMateoBuildingPermits\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -169,9 +169,6 @@
     <t>038121402</t>
   </si>
   <si>
-    <t>ABD-2017-12vdfs</t>
-  </si>
-  <si>
     <t>BD-2018-888889</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>BD-2018-888894</t>
+  </si>
+  <si>
+    <t>BD-2018-777989</t>
   </si>
 </sst>
 </file>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +697,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -759,7 +759,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6">
         <v>43466</v>
@@ -785,7 +785,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>34</v>
@@ -810,7 +810,7 @@
         <v>87654.6</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB2" s="5">
         <v>11000</v>
@@ -833,7 +833,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6">
         <v>43466</v>
@@ -859,7 +859,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>38</v>
@@ -878,13 +878,13 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Z3" s="5">
         <v>900000</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AB3" s="5">
         <v>12000</v>
@@ -907,7 +907,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="6">
         <v>43466</v>
@@ -933,7 +933,7 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>38</v>
@@ -958,7 +958,7 @@
         <v>900000</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AB4" s="5">
         <v>12000</v>
@@ -981,7 +981,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="6">
         <v>43466</v>
@@ -1007,7 +1007,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>38</v>
@@ -1029,10 +1029,10 @@
         <v>0</v>
       </c>
       <c r="Z5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA5" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AB5" s="8">
         <v>10000</v>
@@ -1055,7 +1055,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="9">
         <v>43133</v>
@@ -1081,7 +1081,7 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>38</v>
@@ -1106,7 +1106,7 @@
         <v>3100000</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB6" s="8">
         <v>10000</v>
@@ -1129,7 +1129,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="9">
         <v>43133</v>
@@ -1155,7 +1155,7 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>38</v>
@@ -1180,10 +1180,10 @@
         <v>900000</v>
       </c>
       <c r="AA7" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB7" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC7" s="7" t="s">
         <v>44</v>
@@ -1203,7 +1203,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="9">
         <v>43133</v>
@@ -1229,7 +1229,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>38</v>
@@ -1254,7 +1254,7 @@
         <v>900000</v>
       </c>
       <c r="AA8" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB8" s="12">
         <v>3100000</v>

</xml_diff>